<commit_message>
Added header to output file
</commit_message>
<xml_diff>
--- a/sampleout.xlsx
+++ b/sampleout.xlsx
@@ -14,7 +14,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Venue</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>FS Initials</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
   <si>
     <t>Tue</t>
   </si>
@@ -408,7 +435,7 @@
     <s:outlinePr summaryBelow="1" summaryRight="1"/>
     <s:pageSetUpPr/>
   </s:sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -416,648 +443,677 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="n">
-        <v>42255</v>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="n">
-        <v>0.8125</v>
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>42255</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0.8125</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>42256</v>
+        <v>42255</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0.8125</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>42257</v>
+        <v>42256</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>0.8125</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>42258</v>
+        <v>42257</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.7916666666666666</v>
+        <v>0.8125</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>42258</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.7916666666666666</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>42258</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0.8333333333333334</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>42259</v>
+        <v>42258</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>42259</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0.5833333333333334</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>42259</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>42259</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>0.8333333333333334</v>
       </c>
       <c r="G11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>42260</v>
+        <v>42259</v>
       </c>
       <c r="C12" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>42260</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>42260</v>
       </c>
       <c r="C14" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F14" s="2" t="n">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>42260</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="2" t="n">
         <v>0.7708333333333334</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="1" t="n">
+      <c r="B16" s="1" t="n">
         <v>42262</v>
       </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="2" t="n">
-        <v>0.8125</v>
-      </c>
-      <c r="G15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="1" t="n">
-        <v>42263</v>
-      </c>
       <c r="C16" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>0.8125</v>
       </c>
       <c r="G16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>42263</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F17" s="2" t="n">
+        <v>0.8125</v>
+      </c>
+      <c r="G17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>42263</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="2" t="n">
         <v>0.8333333333333334</v>
       </c>
-      <c r="G17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="1" t="n">
-        <v>42264</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="2" t="n">
-        <v>0.8125</v>
-      </c>
       <c r="G18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>42264</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F19" s="2" t="n">
+        <v>0.8125</v>
+      </c>
+      <c r="G19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>42264</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="2" t="n">
         <v>0.8333333333333334</v>
       </c>
-      <c r="G19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="1" t="n">
-        <v>42265</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" s="2" t="n">
-        <v>0.7916666666666666</v>
-      </c>
       <c r="G20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>42265</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.7916666666666666</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>42265</v>
       </c>
       <c r="C22" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F22" s="2" t="n">
         <v>0.8333333333333334</v>
       </c>
       <c r="G22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>42266</v>
+        <v>42265</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>42266</v>
       </c>
       <c r="C24" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F24" s="2" t="n">
         <v>0.5833333333333334</v>
       </c>
       <c r="G24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>42266</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>42266</v>
       </c>
       <c r="C26" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D26" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F26" s="2" t="n">
         <v>0.8333333333333334</v>
       </c>
       <c r="G26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>42267</v>
+        <v>42266</v>
       </c>
       <c r="C27" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>42267</v>
       </c>
       <c r="C28" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F28" s="2" t="n">
+        <v>0.5416666666666666</v>
+      </c>
+      <c r="G28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>42267</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="2" t="n">
         <v>0.7708333333333334</v>
       </c>
-      <c r="G28" t="s">
-        <v>9</v>
+      <c r="G29" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hacked a way to directly add a timedelta to a datetime.time
</commit_message>
<xml_diff>
--- a/sampleout.xlsx
+++ b/sampleout.xlsx
@@ -489,7 +489,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0.8125</v>
+        <v>0.7291666666666666</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -512,7 +512,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0.8125</v>
+        <v>0.7291666666666666</v>
       </c>
       <c r="G3" t="s">
         <v>16</v>
@@ -535,7 +535,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0.8125</v>
+        <v>0.7291666666666666</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
@@ -558,7 +558,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.8125</v>
+        <v>0.7291666666666666</v>
       </c>
       <c r="G5" t="s">
         <v>18</v>
@@ -581,7 +581,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0.7916666666666666</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="G6" t="s">
         <v>22</v>
@@ -604,7 +604,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="G7" t="s">
         <v>23</v>
@@ -627,7 +627,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="G8" t="s">
         <v>18</v>
@@ -650,7 +650,7 @@
         <v>12</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.5</v>
       </c>
       <c r="G9" t="s">
         <v>23</v>
@@ -673,7 +673,7 @@
         <v>12</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.5</v>
       </c>
       <c r="G10" t="s">
         <v>18</v>
@@ -696,7 +696,7 @@
         <v>12</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="G11" t="s">
         <v>23</v>
@@ -719,7 +719,7 @@
         <v>12</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="G12" t="s">
         <v>18</v>
@@ -742,7 +742,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="G13" t="s">
         <v>18</v>
@@ -765,7 +765,7 @@
         <v>12</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.5</v>
       </c>
       <c r="G14" t="s">
         <v>23</v>
@@ -788,7 +788,7 @@
         <v>12</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>0.7708333333333334</v>
+        <v>0.6875</v>
       </c>
       <c r="G15" t="s">
         <v>18</v>
@@ -811,7 +811,7 @@
         <v>12</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>0.8125</v>
+        <v>0.7291666666666666</v>
       </c>
       <c r="G16" t="s">
         <v>18</v>
@@ -834,7 +834,7 @@
         <v>12</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>0.8125</v>
+        <v>0.7291666666666666</v>
       </c>
       <c r="G17" t="s">
         <v>18</v>
@@ -857,7 +857,7 @@
         <v>12</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="G18" t="s">
         <v>23</v>
@@ -880,7 +880,7 @@
         <v>12</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>0.8125</v>
+        <v>0.7291666666666666</v>
       </c>
       <c r="G19" t="s">
         <v>18</v>
@@ -903,7 +903,7 @@
         <v>12</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="G20" t="s">
         <v>23</v>
@@ -926,7 +926,7 @@
         <v>12</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>0.7916666666666666</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="G21" t="s">
         <v>22</v>
@@ -949,7 +949,7 @@
         <v>12</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="G22" t="s">
         <v>23</v>
@@ -972,7 +972,7 @@
         <v>12</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="G23" t="s">
         <v>18</v>
@@ -995,7 +995,7 @@
         <v>12</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.5</v>
       </c>
       <c r="G24" t="s">
         <v>23</v>
@@ -1018,7 +1018,7 @@
         <v>12</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.5</v>
       </c>
       <c r="G25" t="s">
         <v>18</v>
@@ -1041,7 +1041,7 @@
         <v>12</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="G26" t="s">
         <v>23</v>
@@ -1064,7 +1064,7 @@
         <v>12</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="G27" t="s">
         <v>18</v>
@@ -1087,7 +1087,7 @@
         <v>12</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="G28" t="s">
         <v>18</v>
@@ -1110,7 +1110,7 @@
         <v>12</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>0.7708333333333334</v>
+        <v>0.6875</v>
       </c>
       <c r="G29" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
time adjust working for p&g case
</commit_message>
<xml_diff>
--- a/sampleout.xlsx
+++ b/sampleout.xlsx
@@ -494,7 +494,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0.7291666666666666</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -540,7 +540,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0.7291666666666666</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
@@ -563,7 +563,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.7291666666666666</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="G5" t="s">
         <v>18</v>
@@ -632,7 +632,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0.75</v>
+        <v>0.7291666666666666</v>
       </c>
       <c r="G8" t="s">
         <v>18</v>
@@ -678,7 +678,7 @@
         <v>12</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0.5</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="G10" t="s">
         <v>18</v>
@@ -724,7 +724,7 @@
         <v>12</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>0.75</v>
+        <v>0.7291666666666666</v>
       </c>
       <c r="G12" t="s">
         <v>18</v>
@@ -747,7 +747,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.4375</v>
       </c>
       <c r="G13" t="s">
         <v>18</v>
@@ -793,7 +793,7 @@
         <v>12</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>0.6875</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G15" t="s">
         <v>18</v>
@@ -816,7 +816,7 @@
         <v>12</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>0.7291666666666666</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="G16" t="s">
         <v>18</v>
@@ -839,7 +839,7 @@
         <v>12</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>0.7291666666666666</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="G17" t="s">
         <v>18</v>
@@ -885,7 +885,7 @@
         <v>12</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>0.7291666666666666</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="G19" t="s">
         <v>18</v>
@@ -977,7 +977,7 @@
         <v>12</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>0.75</v>
+        <v>0.7291666666666666</v>
       </c>
       <c r="G23" t="s">
         <v>18</v>
@@ -1023,7 +1023,7 @@
         <v>12</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>0.5</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="G25" t="s">
         <v>18</v>
@@ -1069,7 +1069,7 @@
         <v>12</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>0.75</v>
+        <v>0.7291666666666666</v>
       </c>
       <c r="G27" t="s">
         <v>18</v>
@@ -1092,7 +1092,7 @@
         <v>12</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.4375</v>
       </c>
       <c r="G28" t="s">
         <v>18</v>
@@ -1115,7 +1115,7 @@
         <v>12</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>0.6875</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G29" t="s">
         <v>18</v>

</xml_diff>